<commit_message>
CAMBIO DE COLORES DE GRUPO
</commit_message>
<xml_diff>
--- a/integrantes.xlsx
+++ b/integrantes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LDMM\Documents\GitHub\Modelo_Jonathan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB-8\Documents\modelo_dayana\modelo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
   <si>
     <t>ITEM</t>
   </si>
@@ -318,13 +318,16 @@
   </si>
   <si>
     <t>reingresos</t>
+  </si>
+  <si>
+    <t>ASISTENCIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,8 +342,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,6 +398,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -402,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -413,6 +434,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,7 +744,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +779,7 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="9"/>
@@ -1003,7 +1027,7 @@
       <c r="A29" s="2">
         <v>5</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="3">
@@ -1072,7 +1096,7 @@
       <c r="A37" s="2">
         <v>6</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D37" s="6">
@@ -1123,7 +1147,7 @@
       <c r="A43" s="2">
         <v>7</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D43" s="6">
@@ -1283,6 +1307,12 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>11</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="D63">
         <f>SUM(D2:D62)</f>
         <v>38</v>

</xml_diff>